<commit_message>
Add missing characters to FFIX
</commit_message>
<xml_diff>
--- a/Assets/Exports/FF IX.xlsx
+++ b/Assets/Exports/FF IX.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Zidane</t>
   </si>
@@ -37,6 +37,15 @@
     <t>Amarant</t>
   </si>
   <si>
+    <t>Quina</t>
+  </si>
+  <si>
+    <t>Kuja</t>
+  </si>
+  <si>
+    <t>Beatrix</t>
+  </si>
+  <si>
     <t>Thief</t>
   </si>
   <si>
@@ -55,13 +64,16 @@
     <t>Ninja</t>
   </si>
   <si>
+    <t>Oracle</t>
+  </si>
+  <si>
     <t>Calculator</t>
   </si>
   <si>
     <t>Squire</t>
   </si>
   <si>
-    <t>Dragoner</t>
+    <t>Samurai</t>
   </si>
   <si>
     <t>Mediator</t>
@@ -70,6 +82,12 @@
     <t>Monk</t>
   </si>
   <si>
+    <t>Time Mage</t>
+  </si>
+  <si>
+    <t>Priest</t>
+  </si>
+  <si>
     <t>Two Swords</t>
   </si>
   <si>
@@ -88,6 +106,9 @@
     <t>Martial Arts</t>
   </si>
   <si>
+    <t>Secret Hunt</t>
+  </si>
+  <si>
     <t>Abandon</t>
   </si>
   <si>
@@ -100,9 +121,21 @@
     <t>Speed Save</t>
   </si>
   <si>
+    <t>Counter</t>
+  </si>
+  <si>
     <t>Sunken State</t>
   </si>
   <si>
+    <t>Dragon Spirit</t>
+  </si>
+  <si>
+    <t>Counter Magic</t>
+  </si>
+  <si>
+    <t>Regenerator</t>
+  </si>
+  <si>
     <t>Move +3</t>
   </si>
   <si>
@@ -112,12 +145,21 @@
     <t>Move-HP Up</t>
   </si>
   <si>
+    <t>Ignore Height</t>
+  </si>
+  <si>
+    <t>Walk on Water</t>
+  </si>
+  <si>
     <t>Teleport</t>
   </si>
   <si>
     <t>Gained JP Up: (Squire - 250 JP)</t>
   </si>
   <si>
+    <t>Accumulate: (Squire - 300 JP)</t>
+  </si>
+  <si>
     <t>Move +1: (Squire - 200 JP)</t>
   </si>
   <si>
@@ -133,9 +175,15 @@
     <t>Master Priest! (5,510 JP)</t>
   </si>
   <si>
+    <t>3 Knight</t>
+  </si>
+  <si>
     <t>2 Priest</t>
   </si>
   <si>
+    <t>Magic Attack Up: (Wizard - 400 JP)</t>
+  </si>
+  <si>
     <t>3 Archer</t>
   </si>
   <si>
@@ -145,7 +193,7 @@
     <t>Master Squire! (620 JP)</t>
   </si>
   <si>
-    <t>Master Dragoner! (2,300 JP)</t>
+    <t>Counter: (Monk - 300 JP)</t>
   </si>
   <si>
     <t>Move-MP Up: (Oracle - 350 JP)</t>
@@ -154,13 +202,16 @@
     <t>2 Knight</t>
   </si>
   <si>
+    <t>Counter Magic: (Wizard - 800 JP)</t>
+  </si>
+  <si>
     <t>4 Thief</t>
   </si>
   <si>
     <t>Master Wizard! (6,890 JP)</t>
   </si>
   <si>
-    <t>3 Knight</t>
+    <t>4 Monk</t>
   </si>
   <si>
     <t>2 Oracle</t>
@@ -169,13 +220,13 @@
     <t>Master Monk! (2,700 JP)</t>
   </si>
   <si>
-    <t>Magic Attack Up: (Wizard - 400 JP)</t>
+    <t>2 Wizard</t>
   </si>
   <si>
     <t>Move-HP Up: (Monk - 300 JP)</t>
   </si>
   <si>
-    <t>4 Monk</t>
+    <t>2 Archer</t>
   </si>
   <si>
     <t>Master Mediator! (2,200 JP)</t>
@@ -184,103 +235,226 @@
     <t>Martial Arts: (Monk - 200 JP)</t>
   </si>
   <si>
+    <t>Demi: (Time Mage - 250 JP)</t>
+  </si>
+  <si>
     <t>3 Monk</t>
   </si>
   <si>
     <t>4 Wizard</t>
   </si>
   <si>
+    <t>3 Thief</t>
+  </si>
+  <si>
+    <t>Demi 2: (Time Mage - 550 JP)</t>
+  </si>
+  <si>
+    <t>2 Geomancer</t>
+  </si>
+  <si>
+    <t>Master Time Mage! (5,300 JP)</t>
+  </si>
+  <si>
+    <t>Attack Up: (Geomancer - 400 JP)</t>
+  </si>
+  <si>
+    <t>Ignore Height: (Lancer - 150 JP)</t>
+  </si>
+  <si>
+    <t>Short Charge: (Time Mage - 800 JP)</t>
+  </si>
+  <si>
+    <t>Meteor: (Time Mage - 1,500 JP)</t>
+  </si>
+  <si>
+    <t>Shuriken: (Ninja - 50 JP)</t>
+  </si>
+  <si>
+    <t>MP Switch: (Time Mage - 400 JP)</t>
+  </si>
+  <si>
+    <t>2 Lancer</t>
+  </si>
+  <si>
+    <t>2 Time Mage</t>
+  </si>
+  <si>
+    <t>3 Time Mage</t>
+  </si>
+  <si>
+    <t>Teleport: (Time Mage - 600 JP)</t>
+  </si>
+  <si>
+    <t>Ball: (Ninja - 70 JP)</t>
+  </si>
+  <si>
+    <t>Asura: (Samurai - 100 JP)</t>
+  </si>
+  <si>
+    <t>Master Oracle! (4,670 JP)</t>
+  </si>
+  <si>
+    <t>Bolt: (Wizard - 50 JP)</t>
+  </si>
+  <si>
+    <t>Two Swords: (Ninja - 900 JP)</t>
+  </si>
+  <si>
+    <t>Bizen Boat: (Samurai - 260 JP)</t>
+  </si>
+  <si>
+    <t>Titan: (Summoner - 220 JP)</t>
+  </si>
+  <si>
+    <t>Sunken State: (Ninja - 900 JP)</t>
+  </si>
+  <si>
+    <t>3 Oracle</t>
+  </si>
+  <si>
+    <t>Bolt 2: (Wizard - 200 JP)</t>
+  </si>
+  <si>
+    <t>Two Hands: (Samurai - 900 JP)</t>
+  </si>
+  <si>
+    <t>Abandon: (Ninja - 400 JP)</t>
+  </si>
+  <si>
+    <t>Murasame: (Samurai - 340 JP)</t>
+  </si>
+  <si>
+    <t>Golem: (Summoner - 500 JP)</t>
+  </si>
+  <si>
+    <t>Level: (Calculator - 350 JP)</t>
+  </si>
+  <si>
+    <t>Bolt 3: (Wizard - 480 JP)</t>
+  </si>
+  <si>
+    <t>Regenerator: (Priest - 400 JP)</t>
+  </si>
+  <si>
+    <t>Damage Split: (Calculator - 300 JP)</t>
+  </si>
+  <si>
+    <t>Muramasa: (Samurai - 580 JP)</t>
+  </si>
+  <si>
+    <t>Carbuncle: (Summoner - 350 JP)</t>
+  </si>
+  <si>
+    <t>5: (Calculator - 200 JP)</t>
+  </si>
+  <si>
+    <t>Bolt 4: (Wizard - 850 JP)</t>
+  </si>
+  <si>
+    <t>Master Knight! (2,400 JP)</t>
+  </si>
+  <si>
+    <t>Master Calculator! (2,550 JP)</t>
+  </si>
+  <si>
+    <t>Masamune: (Samurai - 740 JP)</t>
+  </si>
+  <si>
+    <t>Salamander: (Summoner - 820 JP)</t>
+  </si>
+  <si>
+    <t>4 Summoner</t>
+  </si>
+  <si>
+    <t>4: (Calculator - 400 JP)</t>
+  </si>
+  <si>
+    <t>Flare: (Wizard - 900 JP)</t>
+  </si>
+  <si>
     <t>Speed Save: (Archer - 800 JP)</t>
   </si>
   <si>
-    <t>2 Wizard</t>
-  </si>
-  <si>
-    <t>2 Geomancer</t>
-  </si>
-  <si>
-    <t>Master Time Mage! (5,300 JP)</t>
-  </si>
-  <si>
-    <t>Attack Up: (Geomancer - 400 JP)</t>
-  </si>
-  <si>
-    <t>2 Archer</t>
-  </si>
-  <si>
-    <t>Short Charge: (Time Mage - 800 JP)</t>
-  </si>
-  <si>
-    <t>Shuriken: (Ninja - 50 JP)</t>
-  </si>
-  <si>
-    <t>MP Switch: (Time Mage - 400 JP)</t>
-  </si>
-  <si>
-    <t>2 Thief</t>
-  </si>
-  <si>
-    <t>2 Time Mage</t>
-  </si>
-  <si>
-    <t>Ball: (Ninja - 70 JP)</t>
-  </si>
-  <si>
-    <t>3 Time Mage</t>
-  </si>
-  <si>
-    <t>2 Lancer</t>
-  </si>
-  <si>
-    <t>Two Swords: (Ninja - 900 JP)</t>
-  </si>
-  <si>
-    <t>Master Oracle! (4,670 JP)</t>
-  </si>
-  <si>
-    <t>Two Hands: (Samurai - 900 JP)</t>
-  </si>
-  <si>
-    <t>Master Summoner! (7,950 JP)</t>
-  </si>
-  <si>
-    <t>Sunken State: (Ninja - 900 JP)</t>
-  </si>
-  <si>
-    <t>Abandon: (Ninja - 400 JP)</t>
-  </si>
-  <si>
-    <t>3 Oracle</t>
-  </si>
-  <si>
-    <t>Damage Split: (Calculator - 300 JP)</t>
-  </si>
-  <si>
-    <t>Teleport: (Time Mage - 600 JP)</t>
-  </si>
-  <si>
-    <t>Master Calculator! (2,550 JP)</t>
-  </si>
-  <si>
-    <t>Master Knight! (2,400 JP)</t>
+    <t>Silf: (Summoner - 400 JP)</t>
+  </si>
+  <si>
+    <t>3: (Calculator - 600 JP)</t>
+  </si>
+  <si>
+    <t>Moogle: (Summoner - 110 JP)</t>
   </si>
   <si>
     <t>Master Lancer! (5,400 JP)</t>
   </si>
   <si>
-    <t>4 Summoner</t>
+    <t>Cyclops: (Summoner - 1,000 JP)</t>
+  </si>
+  <si>
+    <t>Shiva: (Summoner - 200 JP)</t>
+  </si>
+  <si>
+    <t>Zodiac: (Summoner - 0 JP)</t>
   </si>
   <si>
     <t>4 Mediator</t>
   </si>
   <si>
+    <t>Secret Hunt: (Thief - 200 JP)</t>
+  </si>
+  <si>
+    <t>Ramuh: (Summoner - 200 JP)</t>
+  </si>
+  <si>
     <t>Move +3: (Bard - 1,000 JP)</t>
   </si>
   <si>
+    <t>Ifrit: (Summoner - 200 JP)</t>
+  </si>
+  <si>
     <t>Master Ninja! (1,120 JP)</t>
   </si>
   <si>
+    <t>Dragon Spirit: (Lancer - 560 JP)</t>
+  </si>
+  <si>
     <t>Master Thief! (2,660 JP)</t>
+  </si>
+  <si>
+    <t>Bahamut: (Summoner - 1,200 JP)</t>
+  </si>
+  <si>
+    <t>Odin: (Summoner - 900 JP)</t>
+  </si>
+  <si>
+    <t>Leviathan: (Summoner - 850 JP)</t>
+  </si>
+  <si>
+    <t>Fairy: (Summoner - 400 JP)</t>
+  </si>
+  <si>
+    <t>Walk on Water: (Samurai - 300 JP)</t>
+  </si>
+  <si>
+    <t>Lich: (Summoner - 600 JP)</t>
+  </si>
+  <si>
+    <t>Blind: (Oracle - 100 JP)</t>
+  </si>
+  <si>
+    <t>Silence Song: (Oracle - 170 JP)</t>
+  </si>
+  <si>
+    <t>Confusion Song: (Oracle - 400 JP)</t>
+  </si>
+  <si>
+    <t>Paralyze: (Oracle - 100 JP)</t>
+  </si>
+  <si>
+    <t>Sleep: (Oracle - 350 JP)</t>
+  </si>
+  <si>
+    <t>Petrify: (Oracle - 600 JP)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +819,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -673,120 +847,174 @@
       <c r="T1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="AC3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" t="s">
         <v>17</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="T5" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="W5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="T6" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="W6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="Q7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="T7" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="W7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -794,43 +1022,61 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="J9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="M9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="P9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="S9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="V9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -838,43 +1084,61 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="P10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="V10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -882,43 +1146,61 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="J11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="P11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="S11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>35</v>
+        <v>48</v>
+      </c>
+      <c r="V11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -926,43 +1208,61 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="M12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="P12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q12" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="S12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="V12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13">
@@ -970,43 +1270,61 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="J13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="M13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="P13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q13" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="S13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="V13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -1014,43 +1332,61 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="M14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="P14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q14" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="S14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="V14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -1058,43 +1394,61 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="M15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="P15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="S15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>50</v>
+        <v>61</v>
+      </c>
+      <c r="V15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -1102,43 +1456,61 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="M16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>66</v>
+      </c>
+      <c r="S16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="s">
         <v>53</v>
-      </c>
-      <c r="P16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>54</v>
-      </c>
-      <c r="S16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17">
@@ -1146,43 +1518,61 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="J17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="M17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="P17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="S17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+      <c r="V17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -1190,43 +1580,61 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="J18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="P18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q18" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>40</v>
+        <v>74</v>
+      </c>
+      <c r="V18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19">
@@ -1234,43 +1642,61 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="G19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="J19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="M19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="P19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q19" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="S19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="V19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -1278,13 +1704,13 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="G20" s="2" t="b">
         <v>0</v>
@@ -1296,25 +1722,43 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="M20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="P20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="S20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="V20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W20" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21">
@@ -1322,43 +1766,61 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="G21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="M21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="P21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q21" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="S21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="V21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W21" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22">
@@ -1366,37 +1828,61 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="G22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="J22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="M22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="P22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>96</v>
       </c>
       <c r="S22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T22" t="s">
-        <v>59</v>
+        <v>97</v>
+      </c>
+      <c r="V22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W22" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23">
@@ -1404,31 +1890,37 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="J23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="M23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>80</v>
+        <v>102</v>
+      </c>
+      <c r="P23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>103</v>
       </c>
       <c r="S23" s="2" t="b">
         <v>0</v>
@@ -1436,6 +1928,24 @@
       <c r="T23" t="s">
         <v>68</v>
       </c>
+      <c r="V23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W23" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="b">
@@ -1448,31 +1958,55 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="G24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="M24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>83</v>
+        <v>108</v>
+      </c>
+      <c r="P24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>109</v>
       </c>
       <c r="S24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T24" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="V24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -1480,25 +2014,55 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>113</v>
+      </c>
+      <c r="G25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>112</v>
       </c>
       <c r="J25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>58</v>
+        <v>113</v>
+      </c>
+      <c r="M25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>114</v>
+      </c>
+      <c r="P25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>115</v>
       </c>
       <c r="S25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T25" t="s">
-        <v>39</v>
+        <v>116</v>
+      </c>
+      <c r="V25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W25" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26">
@@ -1506,19 +2070,43 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>116</v>
+      </c>
+      <c r="D26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
       </c>
       <c r="J26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>75</v>
+        <v>119</v>
+      </c>
+      <c r="M26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>100</v>
+      </c>
+      <c r="P26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>120</v>
       </c>
       <c r="S26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T26" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="V26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="27">
@@ -1526,13 +2114,37 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="J27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>123</v>
+      </c>
+      <c r="P27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>124</v>
       </c>
       <c r="S27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T27" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="V27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28">
@@ -1540,13 +2152,31 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="J28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>125</v>
+      </c>
+      <c r="P28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>126</v>
       </c>
       <c r="S28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T28" t="s">
-        <v>86</v>
+        <v>127</v>
+      </c>
+      <c r="V28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -1554,13 +2184,25 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>127</v>
+      </c>
+      <c r="J29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>129</v>
       </c>
       <c r="S29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T29" t="s">
-        <v>87</v>
+        <v>130</v>
+      </c>
+      <c r="V29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W29" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30">
@@ -1568,7 +2210,147 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>130</v>
+      </c>
+      <c r="J30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>131</v>
+      </c>
+      <c r="S30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30" t="s">
+        <v>132</v>
+      </c>
+      <c r="V30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="J31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>135</v>
+      </c>
+      <c r="V31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="J32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>136</v>
+      </c>
+      <c r="V32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="J33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>137</v>
+      </c>
+      <c r="V33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="J34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>138</v>
+      </c>
+      <c r="V34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="J35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>140</v>
+      </c>
+      <c r="V35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="J36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>126</v>
+      </c>
+      <c r="V36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="V37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="V38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="V39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="V40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W40" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>